<commit_message>
Fix test case, fix Testcase group method
</commit_message>
<xml_diff>
--- a/src/test/resources/ComplicatedWorkbook.xlsx
+++ b/src/test/resources/ComplicatedWorkbook.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/phong/Projects/flexcel/src/test/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FFB95D7-664C-7344-A506-1FC7F1C91FBB}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0BFA7F0-6F00-AC44-AE08-C4E61A6B965C}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="360" yWindow="1400" windowWidth="34420" windowHeight="17440" xr2:uid="{B9E8E27A-E728-EC40-9C2D-D38A65C944C3}"/>
   </bookViews>
@@ -121,7 +121,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="457" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="452" uniqueCount="124">
   <si>
     <t>Project Name</t>
   </si>
@@ -589,7 +589,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -612,11 +612,48 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
@@ -650,6 +687,15 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1111,7 +1157,7 @@
   <dimension ref="A3:M42"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1224,24 +1270,14 @@
       <c r="F6" s="10" t="s">
         <v>74</v>
       </c>
-      <c r="G6" s="9" t="s">
+      <c r="G6" s="21" t="s">
         <v>75</v>
       </c>
-      <c r="H6" s="9" t="s">
-        <v>75</v>
-      </c>
-      <c r="I6" s="9" t="s">
-        <v>75</v>
-      </c>
-      <c r="J6" s="9" t="s">
-        <v>75</v>
-      </c>
-      <c r="K6" s="9" t="s">
-        <v>75</v>
-      </c>
-      <c r="L6" s="9" t="s">
-        <v>75</v>
-      </c>
+      <c r="H6" s="22"/>
+      <c r="I6" s="22"/>
+      <c r="J6" s="22"/>
+      <c r="K6" s="22"/>
+      <c r="L6" s="23"/>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A7" s="11" t="s">
@@ -1265,7 +1301,9 @@
       <c r="G7" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="H7" s="1"/>
+      <c r="H7" s="1" t="s">
+        <v>20</v>
+      </c>
       <c r="I7" s="1" t="s">
         <v>81</v>
       </c>
@@ -1275,8 +1313,8 @@
       <c r="K7" s="14" t="s">
         <v>80</v>
       </c>
-      <c r="L7" s="1" t="s">
-        <v>82</v>
+      <c r="L7" s="1">
+        <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.2">
@@ -1310,8 +1348,8 @@
       <c r="K8" s="15" t="s">
         <v>84</v>
       </c>
-      <c r="L8" s="1" t="s">
-        <v>82</v>
+      <c r="L8" s="1">
+        <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.2">
@@ -1424,7 +1462,9 @@
       <c r="K16" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="L16" s="1"/>
+      <c r="L16" s="1" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B17" s="1">
@@ -1847,6 +1887,9 @@
       </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="G6:L6"/>
+  </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
 </worksheet>
@@ -1881,7 +1924,7 @@
       </c>
       <c r="F1" s="2">
         <f ca="1">TODAY()</f>
-        <v>43618</v>
+        <v>43619</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.2">
@@ -2823,7 +2866,7 @@
       </c>
       <c r="F1" s="2">
         <f ca="1">TODAY()</f>
-        <v>43618</v>
+        <v>43619</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.2">

</xml_diff>